<commit_message>
move to  esp32 - dry run (#7)
* import html

* PCB

* compatibility esp32

* porting

* mqtt

* mqtt publish-work

* fire param

* include graph

* /info page

* plot real time

* plot saved graph, crash at 100 readings

* send data to graph, pthread

* send graph data when page loads

* fix surface load

* store data with time, also graphSend

* fix html error and size

* DBG tidy up

* status display on index

* fix crash on portal

* notify

* replace blynk.log

* papertrail printf

* clean update

* espressif32@3.5.0 checkout

* todo button off

* send temperature and fix interval

* restart safety timer

* clean up

* clear warnings

* recover crash from SPIFFS

* send power to index

* print RSSI on info
</commit_message>
<xml_diff>
--- a/wire_calc.xlsx
+++ b/wire_calc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\untrol.io\10. Open Source\kiln\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PERSONAL\kiln\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F26FE3-F4E6-4172-BC2A-358C4149F4FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F7F163-489F-477E-949F-E5F65B54DAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{57B4FE52-0AB1-46A3-8CCE-FD1E2EED1BB4}"/>
   </bookViews>
@@ -207,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -229,6 +229,11 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -635,17 +640,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4931CC22-C8AE-4825-8320-DD0EF59F1B4D}">
-  <dimension ref="A1:T32"/>
+  <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -669,14 +674,14 @@
         <v>9</v>
       </c>
       <c r="C1" s="12">
-        <f>(2*3.14*(325/2))*3</f>
-        <v>3061.5</v>
+        <f>304*4*3</f>
+        <v>3648</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
       </c>
       <c r="E1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F1" s="18">
         <v>10</v>
@@ -776,16 +781,16 @@
         <v>10.849056603773585</v>
       </c>
       <c r="D4" s="7">
-        <f>2300/(2*3.14*A4/2*C4*10)</f>
-        <v>7.5017692852087752</v>
+        <f>2300/(2*PI()*A4/2*C4*10)</f>
+        <v>7.497966207884847</v>
       </c>
       <c r="E4" s="15">
         <f>($E$1-A4) * 3.14 / SQRT((C4*1000 / $C$1)^2 - 1)</f>
-        <v>4.7104372842216344</v>
+        <v>7.9598484067843041</v>
       </c>
       <c r="F4" s="13">
         <f>E4/A4</f>
-        <v>5.2338192046907048</v>
+        <v>8.8442760075381148</v>
       </c>
       <c r="H4" s="5">
         <v>0.9</v>
@@ -821,11 +826,11 @@
       </c>
       <c r="S4" s="15">
         <f t="shared" ref="S4:S14" si="2">($E$1-O4) * 3.14 / SQRT((Q4*1000 / $C$1)^2 - 1)</f>
-        <v>3.7432983625551985</v>
+        <v>6.2820679557114092</v>
       </c>
       <c r="T4" s="13">
         <f t="shared" ref="T4:T14" si="3">S4/O4</f>
-        <v>4.1592204028391091</v>
+        <v>6.9800755063460098</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -840,16 +845,16 @@
         <v>13.372093023255815</v>
       </c>
       <c r="D5" s="7">
-        <f t="shared" ref="D5:D14" si="5">2300/(2*3.14*A5/2*C5*10)</f>
-        <v>5.4777070063694264</v>
+        <f t="shared" ref="D5:D14" si="5">2300/(2*PI()*A5/2*C5*10)</f>
+        <v>5.4749300423611995</v>
       </c>
       <c r="E5" s="15">
         <f t="shared" ref="E5:E14" si="6">($E$1-A5) * 3.14 / SQRT((C5*1000 / $C$1)^2 - 1)</f>
-        <v>3.6925452836971608</v>
+        <v>6.2327111548255472</v>
       </c>
       <c r="F5" s="13">
         <f t="shared" ref="F5:F14" si="7">E5/A5</f>
-        <v>3.6925452836971608</v>
+        <v>6.2327111548255472</v>
       </c>
       <c r="H5" s="5">
         <v>1</v>
@@ -867,11 +872,11 @@
       </c>
       <c r="L5" s="15">
         <f t="shared" ref="L5:L14" si="10">($E$1-H5) * 3.14 / SQRT((J5*1000 / $C$1)^2 - 1)</f>
-        <v>3.9889783948116251</v>
+        <v>6.7464732485998908</v>
       </c>
       <c r="M5" s="13">
         <f t="shared" ref="M5:M14" si="11">L5/H5</f>
-        <v>3.9889783948116251</v>
+        <v>6.7464732485998908</v>
       </c>
       <c r="O5" s="5">
         <v>1</v>
@@ -889,11 +894,11 @@
       </c>
       <c r="S5" s="15">
         <f t="shared" si="2"/>
-        <v>2.9558654092140126</v>
+        <v>4.9680861372843044</v>
       </c>
       <c r="T5" s="13">
         <f t="shared" si="3"/>
-        <v>2.9558654092140126</v>
+        <v>4.9680861372843044</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -909,15 +914,15 @@
       </c>
       <c r="D6" s="7">
         <f t="shared" si="5"/>
-        <v>4.1111754487550654</v>
+        <v>4.1090912580089336</v>
       </c>
       <c r="E6" s="15">
         <f t="shared" si="6"/>
-        <v>2.9615588509469051</v>
+        <v>5.0083916798153325</v>
       </c>
       <c r="F6" s="13">
         <f t="shared" si="7"/>
-        <v>2.6923262281335498</v>
+        <v>4.5530833452866659</v>
       </c>
       <c r="H6" s="5">
         <v>1.1000000000000001</v>
@@ -935,11 +940,11 @@
       </c>
       <c r="L6" s="15">
         <f t="shared" si="10"/>
-        <v>3.2005312065248286</v>
+        <v>5.4197196492334285</v>
       </c>
       <c r="M6" s="13">
         <f t="shared" si="11"/>
-        <v>2.9095738241134801</v>
+        <v>4.9270178629394801</v>
       </c>
       <c r="O6" s="5">
         <v>1.1000000000000001</v>
@@ -975,15 +980,15 @@
       </c>
       <c r="D7" s="7">
         <f t="shared" si="5"/>
-        <v>3.1581740976645429</v>
+        <v>3.1565730379892574</v>
       </c>
       <c r="E7" s="15">
         <f t="shared" si="6"/>
-        <v>2.417920908473568</v>
+        <v>4.10383050600612</v>
       </c>
       <c r="F7" s="13">
         <f t="shared" si="7"/>
-        <v>2.01493409039464</v>
+        <v>3.4198587550051003</v>
       </c>
       <c r="H7" s="5">
         <v>1.2</v>
@@ -1001,11 +1006,11 @@
       </c>
       <c r="L7" s="15">
         <f t="shared" si="10"/>
-        <v>2.6060585221903061</v>
+        <v>4.4270589891252055</v>
       </c>
       <c r="M7" s="13">
         <f t="shared" si="11"/>
-        <v>2.1717154351585886</v>
+        <v>3.6892158242710047</v>
       </c>
       <c r="O7" s="5">
         <v>1.2</v>
@@ -1023,11 +1028,11 @@
       </c>
       <c r="S7" s="15">
         <f t="shared" si="2"/>
-        <v>1.9501116683643756</v>
+        <v>3.3035382913400047</v>
       </c>
       <c r="T7" s="13">
         <f t="shared" si="3"/>
-        <v>1.625093056970313</v>
+        <v>2.7529485761166708</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1043,15 +1048,15 @@
       </c>
       <c r="D8" s="7">
         <f t="shared" si="5"/>
-        <v>2.4987751102400781</v>
+        <v>2.4975083377497427</v>
       </c>
       <c r="E8" s="15">
         <f t="shared" si="6"/>
-        <v>2.0224336948631887</v>
+        <v>3.4489803617308983</v>
       </c>
       <c r="F8" s="13">
         <f t="shared" si="7"/>
-        <v>1.5557182268178373</v>
+        <v>2.6530618167160753</v>
       </c>
       <c r="H8" s="5">
         <v>1.3</v>
@@ -1069,11 +1074,11 @@
       </c>
       <c r="L8" s="15">
         <f t="shared" si="10"/>
-        <v>2.1641149449238775</v>
+        <v>3.6927266444805373</v>
       </c>
       <c r="M8" s="13">
         <f t="shared" si="11"/>
-        <v>1.6647038037875981</v>
+        <v>2.8405589572927208</v>
       </c>
       <c r="O8" s="5">
         <v>1.3</v>
@@ -1091,11 +1096,11 @@
       </c>
       <c r="S8" s="15">
         <f t="shared" si="2"/>
-        <v>1.6225048550736609</v>
+        <v>2.7630469770913288</v>
       </c>
       <c r="T8" s="13">
         <f t="shared" si="3"/>
-        <v>1.2480806577489698</v>
+        <v>2.1254207516087145</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -1111,15 +1116,15 @@
       </c>
       <c r="D9" s="7">
         <f t="shared" si="5"/>
-        <v>1.9949954504094631</v>
+        <v>1.9939840727370317</v>
       </c>
       <c r="E9" s="15">
         <f t="shared" si="6"/>
-        <v>1.6977470886222414</v>
+        <v>2.9110045219238101</v>
       </c>
       <c r="F9" s="13">
         <f t="shared" si="7"/>
-        <v>1.2126764918730297</v>
+        <v>2.0792889442312932</v>
       </c>
       <c r="H9" s="5">
         <v>1.4</v>
@@ -1137,11 +1142,11 @@
       </c>
       <c r="L9" s="15">
         <f t="shared" si="10"/>
-        <v>1.825517397058892</v>
+        <v>3.1315101070006435</v>
       </c>
       <c r="M9" s="13">
         <f t="shared" si="11"/>
-        <v>1.3039409978992087</v>
+        <v>2.2367929335718881</v>
       </c>
       <c r="O9" s="5">
         <v>1.4</v>
@@ -1159,11 +1164,11 @@
       </c>
       <c r="S9" s="15">
         <f t="shared" si="2"/>
-        <v>1.3673016652555254</v>
+        <v>2.3420141101571224</v>
       </c>
       <c r="T9" s="13">
         <f t="shared" si="3"/>
-        <v>0.97664404661108961</v>
+        <v>1.6728672215408018</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -1179,15 +1184,15 @@
       </c>
       <c r="D10" s="7">
         <f t="shared" si="5"/>
-        <v>1.62208067940552</v>
+        <v>1.6212583536294407</v>
       </c>
       <c r="E10" s="15">
         <f t="shared" si="6"/>
-        <v>1.4444394872930497</v>
+        <v>2.491584164531</v>
       </c>
       <c r="F10" s="13">
         <f t="shared" si="7"/>
-        <v>0.96295965819536644</v>
+        <v>1.6610561096873333</v>
       </c>
       <c r="H10" s="5">
         <v>1.5</v>
@@ -1205,11 +1210,11 @@
       </c>
       <c r="L10" s="15">
         <f t="shared" si="10"/>
-        <v>1.5534620952832925</v>
+        <v>2.6805679628497967</v>
       </c>
       <c r="M10" s="13">
         <f t="shared" si="11"/>
-        <v>1.0356413968555283</v>
+        <v>1.7870453085665312</v>
       </c>
       <c r="O10" s="5">
         <v>1.5</v>
@@ -1227,11 +1232,11 @@
       </c>
       <c r="S10" s="15">
         <f t="shared" si="2"/>
-        <v>1.1644031666022894</v>
+        <v>2.0069880138832348</v>
       </c>
       <c r="T10" s="13">
         <f t="shared" si="3"/>
-        <v>0.77626877773485958</v>
+        <v>1.3379920092554898</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1247,15 +1252,15 @@
       </c>
       <c r="D11" s="7">
         <f t="shared" si="5"/>
-        <v>1.3355891719745221</v>
+        <v>1.3349120851832723</v>
       </c>
       <c r="E11" s="15">
         <f t="shared" si="6"/>
-        <v>1.2389405726533722</v>
+        <v>2.1509618511294608</v>
       </c>
       <c r="F11" s="13">
         <f t="shared" si="7"/>
-        <v>0.77433785790835763</v>
+        <v>1.344351156955913</v>
       </c>
       <c r="H11" s="5">
         <v>1.6</v>
@@ -1273,11 +1278,11 @@
       </c>
       <c r="L11" s="15">
         <f t="shared" si="10"/>
-        <v>1.3320892395319164</v>
+        <v>2.3132914565675056</v>
       </c>
       <c r="M11" s="13">
         <f t="shared" si="11"/>
-        <v>0.83255577470744768</v>
+        <v>1.4458071603546909</v>
       </c>
       <c r="O11" s="5">
         <v>1.6</v>
@@ -1295,11 +1300,11 @@
       </c>
       <c r="S11" s="15">
         <f t="shared" si="2"/>
-        <v>0.99935828584325348</v>
+        <v>1.7339900831939046</v>
       </c>
       <c r="T11" s="13">
         <f t="shared" si="3"/>
-        <v>0.62459892865203337</v>
+        <v>1.0837438019961902</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -1315,15 +1320,15 @@
       </c>
       <c r="D12" s="7">
         <f t="shared" si="5"/>
-        <v>1.1146496815286622</v>
+        <v>1.1140846016432673</v>
       </c>
       <c r="E12" s="15">
         <f t="shared" si="6"/>
-        <v>1.0727236666094806</v>
+        <v>1.8752395626057567</v>
       </c>
       <c r="F12" s="13">
         <f t="shared" si="7"/>
-        <v>0.63101392153498859</v>
+        <v>1.1030820956504452</v>
       </c>
       <c r="H12" s="5">
         <v>1.7</v>
@@ -1341,11 +1346,11 @@
       </c>
       <c r="L12" s="15">
         <f t="shared" si="10"/>
-        <v>1.1526091778620191</v>
+        <v>2.0153019470281763</v>
       </c>
       <c r="M12" s="13">
         <f t="shared" si="11"/>
-        <v>0.67800539874236421</v>
+        <v>1.1854717335459861</v>
       </c>
       <c r="O12" s="5">
         <v>1.7</v>
@@ -1381,15 +1386,15 @@
       </c>
       <c r="D13" s="7">
         <f t="shared" si="5"/>
-        <v>0.93949044585987251</v>
+        <v>0.93901416424218243</v>
       </c>
       <c r="E13" s="15">
         <f t="shared" si="6"/>
-        <v>0.93447443031842925</v>
+        <v>1.6454648624678792</v>
       </c>
       <c r="F13" s="13">
         <f t="shared" si="7"/>
-        <v>0.51915246128801629</v>
+        <v>0.91414714581548839</v>
       </c>
       <c r="H13" s="5">
         <v>1.8</v>
@@ -1407,11 +1412,11 @@
       </c>
       <c r="L13" s="15">
         <f t="shared" si="10"/>
-        <v>1.0034918587486767</v>
+        <v>1.767279806125069</v>
       </c>
       <c r="M13" s="13">
         <f t="shared" si="11"/>
-        <v>0.55749547708259817</v>
+        <v>0.9818221145139272</v>
       </c>
       <c r="O13" s="5">
         <v>1.8</v>
@@ -1429,11 +1434,11 @@
       </c>
       <c r="S13" s="15">
         <f t="shared" si="2"/>
-        <v>0.75254948573070712</v>
+        <v>1.3246315489362959</v>
       </c>
       <c r="T13" s="13">
         <f t="shared" si="3"/>
-        <v>0.41808304762817061</v>
+        <v>0.73590641607571994</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1447,17 +1452,17 @@
         <f t="shared" si="4"/>
         <v>53.488372093023258</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="7">
         <f t="shared" si="5"/>
-        <v>0.6847133757961783</v>
+        <v>0.68436625529514994</v>
       </c>
       <c r="E14" s="17">
         <f t="shared" si="6"/>
-        <v>0.72007390809835603</v>
+        <v>1.287919620948663</v>
       </c>
       <c r="F14" s="14">
         <f t="shared" si="7"/>
-        <v>0.36003695404917802</v>
+        <v>0.64395981047433148</v>
       </c>
       <c r="H14" s="8">
         <v>2</v>
@@ -1475,11 +1480,11 @@
       </c>
       <c r="L14" s="17">
         <f t="shared" si="10"/>
-        <v>0.77385715710905512</v>
+        <v>1.3842642163612082</v>
       </c>
       <c r="M14" s="14">
         <f t="shared" si="11"/>
-        <v>0.38692857855452756</v>
+        <v>0.69213210818060411</v>
       </c>
       <c r="O14" s="8">
         <v>2</v>
@@ -1497,11 +1502,11 @@
       </c>
       <c r="S14" s="17">
         <f t="shared" si="2"/>
-        <v>0.58075010663587334</v>
+        <v>1.0384751886706796</v>
       </c>
       <c r="T14" s="14">
         <f t="shared" si="3"/>
-        <v>0.29037505331793667</v>
+        <v>0.51923759433533978</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -1531,11 +1536,11 @@
       </c>
       <c r="B18">
         <f>230*D18</f>
-        <v>2875</v>
+        <v>3680</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="18">
-        <v>12.5</v>
+        <v>16</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1639,19 +1644,19 @@
       </c>
       <c r="C22" s="7">
         <f>230/$D$18/B22</f>
-        <v>8.6792452830188669</v>
+        <v>6.7806603773584904</v>
       </c>
       <c r="D22" s="7">
-        <f>$B$18/(2*3.14*A22/2*C22*10)</f>
-        <v>11.721514508138714</v>
+        <f>$B$18/(2*PI()*(A22/2)/10*C22*10)</f>
+        <v>191.94793492185207</v>
       </c>
       <c r="E22" s="7">
-        <f>($E$1-A22) * 3.14 / SQRT((C22*1000 / $C$1)^2 - 1)</f>
-        <v>6.0367783875379635</v>
+        <f>(($E$1+2*A22)-A22) * 3.14 / SQRT((C22*1000 / $C$1)^2 - 1)</f>
+        <v>17.836250583830527</v>
       </c>
       <c r="F22" s="13">
         <f>E22/A22</f>
-        <v>6.7075315417088479</v>
+        <v>19.818056204256141</v>
       </c>
       <c r="H22" s="5">
         <v>0.9</v>
@@ -1679,19 +1684,19 @@
       </c>
       <c r="Q22" s="7">
         <f>230/$D$18/P22</f>
-        <v>10.760233918128653</v>
+        <v>8.4064327485380126</v>
       </c>
       <c r="R22" s="7">
         <f t="shared" ref="R22:R32" si="12">2300/(2*3.14*O22/2*Q22*10)</f>
-        <v>7.563694267515924</v>
+        <v>9.68152866242038</v>
       </c>
       <c r="S22" s="15">
         <f t="shared" ref="S22:S32" si="13">($E$1-O22) * 3.14 / SQRT((Q22*1000 / $C$1)^2 - 1)</f>
-        <v>4.7527302841892221</v>
+        <v>10.738347882468386</v>
       </c>
       <c r="T22" s="13">
         <f t="shared" ref="T22:T32" si="14">S22/O22</f>
-        <v>5.2808114268769133</v>
+        <v>11.931497647187095</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
@@ -1702,20 +1707,20 @@
         <v>1.72</v>
       </c>
       <c r="C23" s="7">
-        <f t="shared" ref="C23:C32" si="15">230/$D$18/B23</f>
-        <v>10.697674418604651</v>
+        <f t="shared" ref="C23:C33" si="15">230/$D$18/B23</f>
+        <v>8.3575581395348841</v>
       </c>
       <c r="D23" s="7">
-        <f t="shared" ref="D23:D32" si="16">$B$18/(2*3.14*A23/2*C23*10)</f>
-        <v>8.558917197452228</v>
+        <f t="shared" ref="D23:D33" si="16">$B$18/(2*PI()*(A23/2)/10*C23*10)</f>
+        <v>140.15820908444672</v>
       </c>
       <c r="E23" s="7">
-        <f t="shared" ref="E23:E32" si="17">($E$1-A23) * 3.14 / SQRT((C23*1000 / $C$1)^2 - 1)</f>
-        <v>4.689211359295995</v>
+        <f t="shared" ref="E23:E37" si="17">(($E$1+2*A23)-A23) * 3.14 / SQRT((C23*1000 / $C$1)^2 - 1)</f>
+        <v>13.71026118192608</v>
       </c>
       <c r="F23" s="13">
-        <f t="shared" ref="F23:F32" si="18">E23/A23</f>
-        <v>4.689211359295995</v>
+        <f t="shared" ref="F23:F33" si="18">E23/A23</f>
+        <v>13.71026118192608</v>
       </c>
       <c r="H23" s="5">
         <v>1</v>
@@ -1725,19 +1730,19 @@
       </c>
       <c r="J23" s="7">
         <f>230/$D$18/I23</f>
-        <v>9.9459459459459438</v>
+        <v>7.7702702702702702</v>
       </c>
       <c r="K23" s="7">
         <f t="shared" ref="K23:K32" si="19">$B$18/(2*3.14*H23/2*J23*10)</f>
-        <v>9.2058121019108299</v>
+        <v>15.082802547770701</v>
       </c>
       <c r="L23" s="7">
         <f t="shared" ref="L23:L32" si="20">($E$1-H23) * 3.14 / SQRT((J23*1000 / $C$1)^2 - 1)</f>
-        <v>5.0792946160970489</v>
+        <v>11.687298259536147</v>
       </c>
       <c r="M23" s="13">
         <f t="shared" ref="M23:M32" si="21">L23/H23</f>
-        <v>5.0792946160970489</v>
+        <v>11.687298259536147</v>
       </c>
       <c r="O23" s="5">
         <v>1</v>
@@ -1747,19 +1752,19 @@
       </c>
       <c r="Q23" s="7">
         <f t="shared" ref="Q23:Q32" si="22">230/$D$18/P23</f>
-        <v>13.237410071942445</v>
+        <v>10.341726618705037</v>
       </c>
       <c r="R23" s="7">
         <f t="shared" si="12"/>
-        <v>5.5334394904458595</v>
+        <v>7.0828025477707</v>
       </c>
       <c r="S23" s="15">
         <f t="shared" si="13"/>
-        <v>3.732226603649075</v>
+        <v>8.2859807167093642</v>
       </c>
       <c r="T23" s="13">
         <f t="shared" si="14"/>
-        <v>3.732226603649075</v>
+        <v>8.2859807167093642</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -1771,19 +1776,19 @@
       </c>
       <c r="C24" s="7">
         <f t="shared" si="15"/>
-        <v>12.95774647887324</v>
+        <v>10.123239436619718</v>
       </c>
       <c r="D24" s="7">
         <f t="shared" si="16"/>
-        <v>6.4237116386797899</v>
+        <v>105.19273620502869</v>
       </c>
       <c r="E24" s="7">
         <f t="shared" si="17"/>
-        <v>3.7411377410212148</v>
+        <v>11.038535009005711</v>
       </c>
       <c r="F24" s="13">
         <f t="shared" si="18"/>
-        <v>3.4010343100192859</v>
+        <v>10.035031826368828</v>
       </c>
       <c r="H24" s="5">
         <v>1.1000000000000001</v>
@@ -1793,19 +1798,19 @@
       </c>
       <c r="J24" s="7">
         <f t="shared" ref="J24:J32" si="23">230/$D$18/I24</f>
-        <v>12.026143790849671</v>
+        <v>9.3954248366013076</v>
       </c>
       <c r="K24" s="7">
         <f t="shared" si="19"/>
-        <v>6.9213231036479437</v>
+        <v>11.33989577301679</v>
       </c>
       <c r="L24" s="7">
         <f t="shared" si="20"/>
-        <v>4.0502586856350486</v>
+        <v>9.1285352793546171</v>
       </c>
       <c r="M24" s="13">
         <f t="shared" si="21"/>
-        <v>3.6820533505773168</v>
+        <v>8.2986684357769231</v>
       </c>
       <c r="O24" s="5">
         <v>1.1000000000000001</v>
@@ -1837,19 +1842,19 @@
       </c>
       <c r="C25" s="7">
         <f t="shared" si="15"/>
-        <v>15.46218487394958</v>
+        <v>12.079831932773109</v>
       </c>
       <c r="D25" s="7">
         <f t="shared" si="16"/>
-        <v>4.9346470276008496</v>
+        <v>80.808269772524994</v>
       </c>
       <c r="E25" s="7">
         <f t="shared" si="17"/>
-        <v>3.0445185286524707</v>
+        <v>9.1511759273451414</v>
       </c>
       <c r="F25" s="13">
         <f t="shared" si="18"/>
-        <v>2.5370987738770592</v>
+        <v>7.6259799394542851</v>
       </c>
       <c r="H25" s="5">
         <v>1.2</v>
@@ -1859,19 +1864,19 @@
       </c>
       <c r="J25" s="7">
         <f t="shared" si="23"/>
-        <v>14.374999999999998</v>
+        <v>11.23046875</v>
       </c>
       <c r="K25" s="7">
         <f t="shared" si="19"/>
-        <v>5.3078556263269654</v>
+        <v>8.6963906581740975</v>
       </c>
       <c r="L25" s="7">
         <f t="shared" si="20"/>
-        <v>3.2853148864314892</v>
+        <v>7.333460503545564</v>
       </c>
       <c r="M25" s="13">
         <f t="shared" si="21"/>
-        <v>2.7377624053595744</v>
+        <v>6.1112170862879704</v>
       </c>
       <c r="O25" s="5">
         <v>1.2</v>
@@ -1881,19 +1886,19 @@
       </c>
       <c r="Q25" s="7">
         <f t="shared" si="22"/>
-        <v>19.087136929460581</v>
+        <v>14.91182572614108</v>
       </c>
       <c r="R25" s="7">
         <f t="shared" si="12"/>
-        <v>3.1979830148619959</v>
+        <v>4.0934182590233545</v>
       </c>
       <c r="S25" s="15">
         <f t="shared" si="13"/>
-        <v>2.4491985719540854</v>
+        <v>5.3872047533456868</v>
       </c>
       <c r="T25" s="13">
         <f t="shared" si="14"/>
-        <v>2.0409988099617378</v>
+        <v>4.4893372944547396</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
@@ -1905,19 +1910,19 @@
       </c>
       <c r="C26" s="7">
         <f t="shared" si="15"/>
-        <v>18.03921568627451</v>
+        <v>14.093137254901961</v>
       </c>
       <c r="D26" s="7">
         <f t="shared" si="16"/>
-        <v>3.9043361097501217</v>
+        <v>63.936213446393396</v>
       </c>
       <c r="E26" s="7">
         <f t="shared" si="17"/>
-        <v>2.5415015898213724</v>
+        <v>7.8256356288057916</v>
       </c>
       <c r="F26" s="13">
         <f t="shared" si="18"/>
-        <v>1.9550012229395173</v>
+        <v>6.0197197144659933</v>
       </c>
       <c r="H26" s="5">
         <v>1.3</v>
@@ -1927,19 +1932,19 @@
       </c>
       <c r="J26" s="7">
         <f t="shared" si="23"/>
-        <v>16.880733944954127</v>
+        <v>13.188073394495412</v>
       </c>
       <c r="K26" s="7">
         <f t="shared" si="19"/>
-        <v>4.1722807447329737</v>
+        <v>6.8358647721705035</v>
       </c>
       <c r="L26" s="7">
         <f t="shared" si="20"/>
-        <v>2.7216538042727798</v>
+        <v>6.0556813893126229</v>
       </c>
       <c r="M26" s="13">
         <f t="shared" si="21"/>
-        <v>2.0935798494405997</v>
+        <v>4.6582164533174018</v>
       </c>
       <c r="O26" s="5">
         <v>1.3</v>
@@ -1949,19 +1954,19 @@
       </c>
       <c r="Q26" s="7">
         <f t="shared" si="22"/>
-        <v>22.411693057247259</v>
+        <v>17.509135200974423</v>
       </c>
       <c r="R26" s="7">
         <f t="shared" si="12"/>
-        <v>2.514086232239098</v>
+        <v>3.2180303772660448</v>
       </c>
       <c r="S26" s="15">
         <f t="shared" si="13"/>
-        <v>2.0350609697742783</v>
+        <v>4.4815830605344811</v>
       </c>
       <c r="T26" s="13">
         <f t="shared" si="14"/>
-        <v>1.5654315152109832</v>
+        <v>3.4473715850265236</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
@@ -1973,19 +1978,19 @@
       </c>
       <c r="C27" s="7">
         <f t="shared" si="15"/>
-        <v>20.9806157354618</v>
+        <v>16.391106043329533</v>
       </c>
       <c r="D27" s="7">
         <f t="shared" si="16"/>
-        <v>3.1171803912647862</v>
+        <v>51.045992262068012</v>
       </c>
       <c r="E27" s="7">
         <f t="shared" si="17"/>
-        <v>2.1304782975799776</v>
+        <v>6.7380698847224894</v>
       </c>
       <c r="F27" s="13">
         <f t="shared" si="18"/>
-        <v>1.5217702125571271</v>
+        <v>4.8129070605160642</v>
       </c>
       <c r="H27" s="5">
         <v>1.4</v>
@@ -1995,19 +2000,19 @@
       </c>
       <c r="J27" s="7">
         <f t="shared" si="23"/>
-        <v>19.532908704883226</v>
+        <v>15.260084925690022</v>
       </c>
       <c r="K27" s="7">
         <f t="shared" si="19"/>
-        <v>3.348214285714286</v>
+        <v>5.4857142857142867</v>
       </c>
       <c r="L27" s="7">
         <f t="shared" si="20"/>
-        <v>2.2922178049772644</v>
+        <v>5.1021067316337643</v>
       </c>
       <c r="M27" s="13">
         <f t="shared" si="21"/>
-        <v>1.6372984321266175</v>
+        <v>3.6443619511669749</v>
       </c>
       <c r="O27" s="5">
         <v>1.4</v>
@@ -2017,19 +2022,19 @@
       </c>
       <c r="Q27" s="7">
         <f t="shared" si="22"/>
-        <v>25.988700564971751</v>
+        <v>20.303672316384183</v>
       </c>
       <c r="R27" s="7">
         <f t="shared" si="12"/>
-        <v>2.01319381255687</v>
+        <v>2.5768880800727931</v>
       </c>
       <c r="S27" s="15">
         <f t="shared" si="13"/>
-        <v>1.7134508878094648</v>
+        <v>3.7851178738159899</v>
       </c>
       <c r="T27" s="13">
         <f t="shared" si="14"/>
-        <v>1.2238934912924748</v>
+        <v>2.7036556241542788</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -2041,19 +2046,19 @@
       </c>
       <c r="C28" s="7">
         <f t="shared" si="15"/>
-        <v>24.083769633507853</v>
+        <v>18.815445026178011</v>
       </c>
       <c r="D28" s="7">
         <f t="shared" si="16"/>
-        <v>2.5345010615711252</v>
+        <v>41.504213852913672</v>
       </c>
       <c r="E28" s="7">
         <f t="shared" si="17"/>
-        <v>1.8108794679253912</v>
+        <v>5.8954055740715328</v>
       </c>
       <c r="F28" s="13">
         <f t="shared" si="18"/>
-        <v>1.2072529786169275</v>
+        <v>3.930270382714355</v>
       </c>
       <c r="H28" s="5">
         <v>1.5</v>
@@ -2063,19 +2068,19 @@
       </c>
       <c r="J28" s="7">
         <f t="shared" si="23"/>
-        <v>22.411693057247259</v>
+        <v>17.509135200974423</v>
       </c>
       <c r="K28" s="7">
         <f t="shared" si="19"/>
-        <v>2.7235934182590236</v>
+        <v>4.4623354564755839</v>
       </c>
       <c r="L28" s="7">
         <f t="shared" si="20"/>
-        <v>1.9484626306349475</v>
+        <v>4.3478044617125562</v>
       </c>
       <c r="M28" s="13">
         <f t="shared" si="21"/>
-        <v>1.298975087089965</v>
+        <v>2.8985363078083708</v>
       </c>
       <c r="O28" s="5">
         <v>1.5</v>
@@ -2085,23 +2090,23 @@
       </c>
       <c r="Q28" s="7">
         <f t="shared" si="22"/>
-        <v>29.821717990275523</v>
+        <v>23.298217179902757</v>
       </c>
       <c r="R28" s="7">
         <f t="shared" si="12"/>
-        <v>1.6374734607218688</v>
+        <v>2.095966029723991</v>
       </c>
       <c r="S28" s="15">
         <f t="shared" si="13"/>
-        <v>1.4582918425038385</v>
+        <v>3.2356776876188942</v>
       </c>
       <c r="T28" s="13">
         <f t="shared" si="14"/>
-        <v>0.97219456166922569</v>
+        <v>2.157118458412596</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="23">
         <v>1.6</v>
       </c>
       <c r="B29" s="6">
@@ -2109,19 +2114,19 @@
       </c>
       <c r="C29" s="7">
         <f t="shared" si="15"/>
-        <v>27.421758569299548</v>
+        <v>21.423248882265273</v>
       </c>
       <c r="D29" s="7">
         <f t="shared" si="16"/>
-        <v>2.0868580812101913</v>
+        <v>34.173749380691767</v>
       </c>
       <c r="E29" s="7">
         <f t="shared" si="17"/>
-        <v>1.5521902334721722</v>
+        <v>5.2090662577129345</v>
       </c>
       <c r="F29" s="13">
         <f t="shared" si="18"/>
-        <v>0.97011889592010758</v>
+        <v>3.255666411070584</v>
       </c>
       <c r="H29" s="5">
         <v>1.6</v>
@@ -2131,19 +2136,19 @@
       </c>
       <c r="J29" s="7">
         <f t="shared" si="23"/>
-        <v>25.52011095700416</v>
+        <v>19.937586685159502</v>
       </c>
       <c r="K29" s="7">
         <f t="shared" si="19"/>
-        <v>2.2423616640127384</v>
+        <v>3.6738853503184705</v>
       </c>
       <c r="L29" s="7">
         <f t="shared" si="20"/>
-        <v>1.6694821907475328</v>
+        <v>3.740124656982784</v>
       </c>
       <c r="M29" s="13">
         <f t="shared" si="21"/>
-        <v>1.0434263692172079</v>
+        <v>2.33757791061424</v>
       </c>
       <c r="O29" s="5">
         <v>1.6</v>
@@ -2153,19 +2158,19 @@
       </c>
       <c r="Q29" s="7">
         <f t="shared" si="22"/>
-        <v>33.948339483394832</v>
+        <v>26.522140221402211</v>
       </c>
       <c r="R29" s="7">
         <f t="shared" si="12"/>
-        <v>1.348527070063694</v>
+        <v>1.7261146496815285</v>
       </c>
       <c r="S29" s="15">
         <f t="shared" si="13"/>
-        <v>1.2510401620126335</v>
+        <v>2.7906373198758732</v>
       </c>
       <c r="T29" s="13">
         <f t="shared" si="14"/>
-        <v>0.78190010125789589</v>
+        <v>1.7441483249224206</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
@@ -2177,19 +2182,19 @@
       </c>
       <c r="C30" s="7">
         <f t="shared" si="15"/>
-        <v>30.92436974789916</v>
+        <v>24.159663865546218</v>
       </c>
       <c r="D30" s="7">
         <f t="shared" si="16"/>
-        <v>1.7416401273885351</v>
+        <v>28.520565802067651</v>
       </c>
       <c r="E30" s="7">
         <f t="shared" si="17"/>
-        <v>1.3432914507835434</v>
+        <v>4.6523621519559919</v>
       </c>
       <c r="F30" s="13">
         <f t="shared" si="18"/>
-        <v>0.79017144163737851</v>
+        <v>2.7366836187976422</v>
       </c>
       <c r="H30" s="5">
         <v>1.7</v>
@@ -2199,19 +2204,19 @@
       </c>
       <c r="J30" s="7">
         <f t="shared" si="23"/>
-        <v>28.794992175273862</v>
+        <v>22.496087636932707</v>
       </c>
       <c r="K30" s="7">
         <f t="shared" si="19"/>
-        <v>1.8704336830273511</v>
+        <v>3.0645185462720121</v>
       </c>
       <c r="L30" s="7">
         <f t="shared" si="20"/>
-        <v>1.4437235076994779</v>
+        <v>3.2509076737761973</v>
       </c>
       <c r="M30" s="13">
         <f t="shared" si="21"/>
-        <v>0.84924912217616344</v>
+        <v>1.9122986316330572</v>
       </c>
       <c r="O30" s="5">
         <v>1.7</v>
@@ -2243,19 +2248,19 @@
       </c>
       <c r="C31" s="7">
         <f t="shared" si="15"/>
-        <v>34.651600753295661</v>
+        <v>27.071563088512239</v>
       </c>
       <c r="D31" s="7">
         <f t="shared" si="16"/>
-        <v>1.4679538216560513</v>
+        <v>24.038762604599874</v>
       </c>
       <c r="E31" s="7">
         <f t="shared" si="17"/>
-        <v>1.1697460195647915</v>
+        <v>4.1848178238657958</v>
       </c>
       <c r="F31" s="13">
         <f t="shared" si="18"/>
-        <v>0.64985889975821753</v>
+        <v>2.3248987910365533</v>
       </c>
       <c r="H31" s="5">
         <v>1.8</v>
@@ -2265,19 +2270,19 @@
       </c>
       <c r="J31" s="7">
         <f t="shared" si="23"/>
-        <v>32.280701754385966</v>
+        <v>25.219298245614038</v>
       </c>
       <c r="K31" s="7">
         <f t="shared" si="19"/>
-        <v>1.5757696390658174</v>
+        <v>2.5817409766454351</v>
       </c>
       <c r="L31" s="7">
         <f t="shared" si="20"/>
-        <v>1.2564124399573835</v>
+        <v>2.8460003942346432</v>
       </c>
       <c r="M31" s="13">
         <f t="shared" si="21"/>
-        <v>0.69800691108743529</v>
+        <v>1.5811113301303572</v>
       </c>
       <c r="O31" s="5">
         <v>1.8</v>
@@ -2287,43 +2292,43 @@
       </c>
       <c r="Q31" s="7">
         <f t="shared" si="22"/>
-        <v>42.990654205607477</v>
+        <v>33.586448598130843</v>
       </c>
       <c r="R31" s="7">
         <f t="shared" si="12"/>
-        <v>0.94656758669497532</v>
+        <v>1.2116065109695682</v>
       </c>
       <c r="S31" s="15">
         <f t="shared" si="13"/>
-        <v>0.94154953165089339</v>
+        <v>2.127105634713903</v>
       </c>
       <c r="T31" s="13">
         <f t="shared" si="14"/>
-        <v>0.52308307313938518</v>
+        <v>1.1817253526188349</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="8">
+      <c r="A32" s="5">
         <v>2</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32" s="6">
         <v>0.43</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="7">
         <f t="shared" si="15"/>
-        <v>42.790697674418603</v>
-      </c>
-      <c r="D32" s="10">
+        <v>33.430232558139537</v>
+      </c>
+      <c r="D32" s="7">
         <f t="shared" si="16"/>
-        <v>1.0698646496815285</v>
-      </c>
-      <c r="E32" s="10">
+        <v>17.519776135555841</v>
+      </c>
+      <c r="E32" s="7">
         <f t="shared" si="17"/>
-        <v>0.90092560035919078</v>
-      </c>
-      <c r="F32" s="14">
+        <v>3.4470401378617788</v>
+      </c>
+      <c r="F32" s="13">
         <f t="shared" si="18"/>
-        <v>0.45046280017959539</v>
+        <v>1.7235200689308894</v>
       </c>
       <c r="H32" s="8">
         <v>2</v>
@@ -2333,19 +2338,19 @@
       </c>
       <c r="J32" s="10">
         <f t="shared" si="23"/>
-        <v>39.826839826839823</v>
+        <v>31.114718614718612</v>
       </c>
       <c r="K32" s="10">
         <f t="shared" si="19"/>
-        <v>1.1494824840764331</v>
+        <v>1.8833121019108281</v>
       </c>
       <c r="L32" s="10">
         <f t="shared" si="20"/>
-        <v>0.96835587822445623</v>
+        <v>2.2242083785861997</v>
       </c>
       <c r="M32" s="14">
         <f t="shared" si="21"/>
-        <v>0.48417793911222812</v>
+        <v>1.1121041892930998</v>
       </c>
       <c r="O32" s="8">
         <v>2</v>
@@ -2355,59 +2360,184 @@
       </c>
       <c r="Q32" s="10">
         <f t="shared" si="22"/>
-        <v>53.02593659942363</v>
+        <v>41.426512968299711</v>
       </c>
       <c r="R32" s="10">
         <f t="shared" si="12"/>
-        <v>0.69068471337579618</v>
+        <v>0.88407643312101913</v>
       </c>
       <c r="S32" s="17">
         <f t="shared" si="13"/>
-        <v>0.72637453434493382</v>
+        <v>1.6655120418539189</v>
       </c>
       <c r="T32" s="14">
         <f t="shared" si="14"/>
-        <v>0.36318726717246691</v>
+        <v>0.83275602092695944</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B33" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="C33" s="7">
+        <f t="shared" si="15"/>
+        <v>41.071428571428577</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" si="16"/>
+        <v>12.963893546394381</v>
+      </c>
+      <c r="E33" s="7">
+        <f t="shared" si="17"/>
+        <v>2.8560429893497075</v>
+      </c>
+      <c r="F33" s="13">
+        <f t="shared" si="18"/>
+        <v>1.2982013587953214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="B34" s="6">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="C34" s="7">
+        <f t="shared" ref="C34:C37" si="24">230/$D$18/B34</f>
+        <v>52.272727272727266</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" ref="D34:D37" si="25">$B$18/(2*PI()*(A34/2)/10*C34*10)</f>
+        <v>8.963606394935546</v>
+      </c>
+      <c r="E34" s="7">
+        <f t="shared" si="17"/>
+        <v>2.3065282709331529</v>
+      </c>
+      <c r="F34" s="13">
+        <f t="shared" ref="F34:F37" si="26">E34/A34</f>
+        <v>0.92261130837326122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>3</v>
+      </c>
+      <c r="B35" s="6">
+        <v>0.191</v>
+      </c>
+      <c r="C35" s="19">
+        <f t="shared" si="24"/>
+        <v>75.261780104712045</v>
+      </c>
+      <c r="D35" s="19">
+        <f t="shared" si="25"/>
+        <v>5.188026731614209</v>
+      </c>
+      <c r="E35" s="7">
+        <f t="shared" si="17"/>
+        <v>1.6761521834015676</v>
+      </c>
+      <c r="F35" s="20">
+        <f t="shared" si="26"/>
+        <v>0.55871739446718915</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>4</v>
+      </c>
+      <c r="B36" s="6">
+        <v>0.107</v>
+      </c>
+      <c r="C36" s="19">
+        <f t="shared" si="24"/>
+        <v>134.34579439252337</v>
+      </c>
+      <c r="D36" s="19">
+        <f t="shared" si="25"/>
+        <v>2.1797861005865986</v>
+      </c>
+      <c r="E36" s="7">
+        <f t="shared" si="17"/>
+        <v>1.0235329216538469</v>
+      </c>
+      <c r="F36" s="20">
+        <f t="shared" si="26"/>
+        <v>0.25588323041346173</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="8">
+        <v>5</v>
+      </c>
+      <c r="B37" s="9">
+        <v>6.88E-2</v>
+      </c>
+      <c r="C37" s="21">
+        <f t="shared" si="24"/>
+        <v>208.93895348837211</v>
+      </c>
+      <c r="D37" s="21">
+        <f t="shared" si="25"/>
+        <v>1.1212656726755736</v>
+      </c>
+      <c r="E37" s="7">
+        <f t="shared" si="17"/>
+        <v>0.7128113724833296</v>
+      </c>
+      <c r="F37" s="22">
+        <f t="shared" si="26"/>
+        <v>0.14256227449666592</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4:D14">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:K14">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:K32">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D32">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
+  <conditionalFormatting sqref="D22:D31 D35:D37">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5:R14">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R23:R32">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32:D34">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>